<commit_message>
Menu Administrador - Configuracion - FINALIZADO
</commit_message>
<xml_diff>
--- a/SG - CLASES SEPARADAS/BASE DE DATOS.xlsx
+++ b/SG - CLASES SEPARADAS/BASE DE DATOS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandra\Documents\GitHub\TP-GESTION-PROGRAMACION-2\SG - CLASES SEPARADAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D15BD1F-9451-4AD8-A4D1-71DCB9EA2DF1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A60D6BC0-34FB-4AC8-91FD-E0C007C4600A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="1" activeTab="1" xr2:uid="{A683A0A2-948E-478E-9454-D16ED83D3AB7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="1" activeTab="2" xr2:uid="{A683A0A2-948E-478E-9454-D16ED83D3AB7}"/>
   </bookViews>
   <sheets>
     <sheet name="PRECIO DE COSTO" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="MODIFICACIONES" sheetId="4" r:id="rId3"/>
     <sheet name="AGREGAR COMPRA" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="147">
   <si>
     <t xml:space="preserve">PRECIO </t>
   </si>
@@ -339,9 +339,6 @@
     <t>CONTADOR DE TIQUETS DEBITO/CREDITO</t>
   </si>
   <si>
-    <t>cierre de caja</t>
-  </si>
-  <si>
     <t>CANTIDAD DE NUMEROS NEGATIVOS y 0(corregir leyenda DICE SIEMPRE MAYOR AL STOCK)</t>
   </si>
   <si>
@@ -469,6 +466,9 @@
   </si>
   <si>
     <t>beldent</t>
+  </si>
+  <si>
+    <t>CIERRE DE CAJA</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -753,35 +753,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -852,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -938,9 +909,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -954,17 +922,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -975,26 +935,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1002,49 +962,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1054,50 +1014,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1421,26 +1391,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.375" customWidth="1"/>
-    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.25" customWidth="1"/>
-    <col min="7" max="7" width="10.25" customWidth="1"/>
-    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1524,15 +1494,15 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -1639,972 +1609,975 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABC7CB8-BD08-475E-BF73-5156E3B0BE3D}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.625" style="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.25" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.75" style="43" customWidth="1"/>
-    <col min="4" max="4" width="12" style="43" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5" style="58" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.375" style="58" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" style="42"/>
-    <col min="17" max="16384" width="11" style="43"/>
+    <col min="1" max="1" width="17.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="12" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="53" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="53" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="37"/>
+    <col min="15" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="16384" width="11" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="43"/>
-      <c r="K1" s="42" t="s">
+      <c r="A1" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="38"/>
+      <c r="K1" s="37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="73" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="73" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="50">
+        <v>1</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="38"/>
+      <c r="F3" s="71">
+        <v>1001</v>
+      </c>
+      <c r="G3" s="76" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="78" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="78" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="64" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="64" t="s">
+      <c r="H3" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="60">
+        <v>12</v>
+      </c>
+      <c r="J3" s="60">
         <v>36</v>
       </c>
-      <c r="K2" s="79" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="78" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="78" t="s">
-        <v>81</v>
-      </c>
-      <c r="O2" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="P2" s="78" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="55">
-        <v>1</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="76">
-        <v>1001</v>
-      </c>
-      <c r="G3" s="81" t="s">
-        <v>131</v>
-      </c>
-      <c r="H3" s="76" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="65">
-        <v>12</v>
-      </c>
-      <c r="J3" s="65">
-        <v>36</v>
-      </c>
-      <c r="K3" s="77">
+      <c r="K3" s="72">
         <f>I3*10</f>
         <v>120</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="L3" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="76">
+      <c r="M3" s="71">
         <v>50</v>
       </c>
-      <c r="N3" s="76">
+      <c r="N3" s="71">
         <v>30</v>
       </c>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="47">
+      <c r="A4" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="42">
         <v>2</v>
       </c>
-      <c r="C4" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="59">
+      <c r="C4" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="38"/>
+      <c r="F4" s="54">
         <v>1002</v>
       </c>
-      <c r="G4" s="82" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" s="59" t="s">
+      <c r="G4" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="66">
+      <c r="I4" s="61">
         <v>8</v>
       </c>
-      <c r="J4" s="66">
+      <c r="J4" s="61">
         <v>48</v>
       </c>
-      <c r="K4" s="70">
+      <c r="K4" s="65">
         <f t="shared" ref="K4:K18" si="0">I4*10</f>
         <v>80</v>
       </c>
-      <c r="L4" s="59" t="s">
+      <c r="L4" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="59">
+      <c r="M4" s="54">
         <v>50</v>
       </c>
-      <c r="N4" s="59">
+      <c r="N4" s="54">
         <v>60</v>
       </c>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="47">
+      <c r="A5" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="42">
         <v>3</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="59">
+      <c r="C5" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="38"/>
+      <c r="F5" s="54">
         <v>2001</v>
       </c>
-      <c r="G5" s="82" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="59" t="s">
+      <c r="G5" s="77" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="66">
+      <c r="I5" s="61">
         <v>12</v>
       </c>
-      <c r="J5" s="66">
+      <c r="J5" s="61">
         <v>12</v>
       </c>
-      <c r="K5" s="70">
+      <c r="K5" s="65">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="59">
+      <c r="M5" s="54">
         <v>50</v>
       </c>
-      <c r="N5" s="59">
+      <c r="N5" s="54">
         <v>30</v>
       </c>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="48">
+      <c r="A6" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="43">
         <v>4</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="59">
+      <c r="C6" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="38"/>
+      <c r="F6" s="54">
         <v>2002</v>
       </c>
-      <c r="G6" s="82" t="s">
-        <v>134</v>
-      </c>
-      <c r="H6" s="59" t="s">
+      <c r="G6" s="77" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="66">
+      <c r="I6" s="61">
         <v>6</v>
       </c>
-      <c r="J6" s="66">
+      <c r="J6" s="61">
         <v>6</v>
       </c>
-      <c r="K6" s="70">
+      <c r="K6" s="65">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="L6" s="59" t="s">
+      <c r="L6" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="59">
+      <c r="M6" s="54">
         <v>50</v>
       </c>
-      <c r="N6" s="59">
+      <c r="N6" s="54">
         <v>55</v>
       </c>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="86" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="59">
+      <c r="A7" s="83" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="54">
         <v>3001</v>
       </c>
-      <c r="G7" s="82" t="s">
-        <v>135</v>
-      </c>
-      <c r="H7" s="59" t="s">
+      <c r="G7" s="77" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="66">
+      <c r="I7" s="61">
         <v>20</v>
       </c>
-      <c r="J7" s="66">
+      <c r="J7" s="61">
         <v>20</v>
       </c>
-      <c r="K7" s="70">
+      <c r="K7" s="65">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="L7" s="59" t="s">
+      <c r="L7" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="M7" s="59">
+      <c r="M7" s="54">
         <v>80</v>
       </c>
-      <c r="N7" s="59">
+      <c r="N7" s="54">
         <v>20</v>
       </c>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="69"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="59">
+      <c r="E8" s="38"/>
+      <c r="F8" s="54">
         <v>3002</v>
       </c>
-      <c r="G8" s="82" t="s">
-        <v>136</v>
-      </c>
-      <c r="H8" s="59" t="s">
+      <c r="G8" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="66">
+      <c r="I8" s="61">
         <v>21</v>
       </c>
-      <c r="J8" s="66">
+      <c r="J8" s="61">
         <v>21</v>
       </c>
-      <c r="K8" s="70">
+      <c r="K8" s="65">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
-      <c r="L8" s="62" t="s">
+      <c r="L8" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="59">
+      <c r="M8" s="54">
         <v>80</v>
       </c>
-      <c r="N8" s="59">
+      <c r="N8" s="54">
         <v>20</v>
       </c>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="69"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="46">
+      <c r="A9" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="41">
         <v>34</v>
       </c>
-      <c r="C9" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="59">
+      <c r="C9" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="54">
         <v>3003</v>
       </c>
-      <c r="G9" s="82" t="s">
-        <v>137</v>
-      </c>
-      <c r="H9" s="59" t="s">
+      <c r="G9" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="H9" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="66">
+      <c r="I9" s="61">
         <v>20</v>
       </c>
-      <c r="J9" s="66">
+      <c r="J9" s="61">
         <v>60</v>
       </c>
-      <c r="K9" s="70">
+      <c r="K9" s="65">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="L9" s="59" t="s">
+      <c r="L9" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="59">
+      <c r="M9" s="54">
         <v>80</v>
       </c>
-      <c r="N9" s="59">
+      <c r="N9" s="54">
         <v>15</v>
       </c>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="47">
+      <c r="A10" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="42">
         <v>29</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="47" t="s">
-        <v>120</v>
-      </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="59">
+      <c r="E10" s="38"/>
+      <c r="F10" s="54">
         <v>5001</v>
       </c>
-      <c r="G10" s="82" t="s">
-        <v>138</v>
-      </c>
-      <c r="H10" s="59" t="s">
+      <c r="G10" s="77" t="s">
+        <v>137</v>
+      </c>
+      <c r="H10" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="66">
+      <c r="I10" s="61">
         <v>10</v>
       </c>
-      <c r="J10" s="66">
+      <c r="J10" s="61">
         <v>40</v>
       </c>
-      <c r="K10" s="70">
+      <c r="K10" s="65">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L10" s="59" t="s">
+      <c r="L10" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="M10" s="59">
+      <c r="M10" s="54">
         <v>35</v>
       </c>
-      <c r="N10" s="59">
+      <c r="N10" s="54">
         <v>70</v>
       </c>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="47">
+      <c r="A11" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="42">
         <v>22</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="59">
+      <c r="E11" s="38"/>
+      <c r="F11" s="54">
         <v>5002</v>
       </c>
-      <c r="G11" s="82" t="s">
-        <v>139</v>
-      </c>
-      <c r="H11" s="59" t="s">
+      <c r="G11" s="77" t="s">
+        <v>138</v>
+      </c>
+      <c r="H11" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="66">
+      <c r="I11" s="61">
         <v>10</v>
       </c>
-      <c r="J11" s="66">
+      <c r="J11" s="61">
         <v>20</v>
       </c>
-      <c r="K11" s="70">
+      <c r="K11" s="65">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L11" s="59" t="s">
+      <c r="L11" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="M11" s="59">
+      <c r="M11" s="54">
         <v>35</v>
       </c>
-      <c r="N11" s="59">
+      <c r="N11" s="54">
         <v>70</v>
       </c>
-      <c r="O11" s="74"/>
-      <c r="P11" s="74"/>
+      <c r="O11" s="69"/>
+      <c r="P11" s="69"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" s="47">
+      <c r="A12" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="42">
         <v>60</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="59">
+      <c r="E12" s="38"/>
+      <c r="F12" s="54">
         <v>6001</v>
       </c>
-      <c r="G12" s="82" t="s">
-        <v>140</v>
-      </c>
-      <c r="H12" s="59" t="s">
+      <c r="G12" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="H12" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="66">
+      <c r="I12" s="61">
         <v>10</v>
       </c>
-      <c r="J12" s="66">
+      <c r="J12" s="61">
         <v>60</v>
       </c>
-      <c r="K12" s="70">
+      <c r="K12" s="65">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L12" s="73" t="s">
+      <c r="L12" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="59">
+      <c r="M12" s="54">
         <v>35</v>
       </c>
-      <c r="N12" s="59">
+      <c r="N12" s="54">
         <v>65</v>
       </c>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="69"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="B13" s="47">
+      <c r="A13" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="42">
         <v>19</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D13" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="59">
+      <c r="E13" s="38"/>
+      <c r="F13" s="54">
         <v>6002</v>
       </c>
-      <c r="G13" s="82" t="s">
-        <v>141</v>
-      </c>
-      <c r="H13" s="59" t="s">
+      <c r="G13" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="66">
+      <c r="I13" s="61">
         <v>10</v>
       </c>
-      <c r="J13" s="66">
+      <c r="J13" s="61">
         <v>60</v>
       </c>
-      <c r="K13" s="70">
+      <c r="K13" s="65">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="L13" s="59" t="s">
+      <c r="L13" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="M13" s="59">
+      <c r="M13" s="54">
         <v>35</v>
       </c>
-      <c r="N13" s="59">
+      <c r="N13" s="54">
         <v>70</v>
       </c>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="54"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="48">
+      <c r="A14" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="43">
         <v>21</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D14" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="60">
+      <c r="E14" s="38"/>
+      <c r="F14" s="55">
         <v>8001</v>
       </c>
-      <c r="G14" s="83" t="s">
-        <v>142</v>
-      </c>
-      <c r="H14" s="60" t="s">
+      <c r="G14" s="78" t="s">
+        <v>141</v>
+      </c>
+      <c r="H14" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="67">
+      <c r="I14" s="62">
         <v>12</v>
       </c>
-      <c r="J14" s="69">
+      <c r="J14" s="64">
         <v>24</v>
       </c>
-      <c r="K14" s="71">
+      <c r="K14" s="66">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="L14" s="60" t="s">
+      <c r="L14" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="M14" s="60">
+      <c r="M14" s="55">
         <v>50</v>
       </c>
-      <c r="N14" s="60">
+      <c r="N14" s="55">
         <v>25</v>
       </c>
-      <c r="O14" s="71"/>
-      <c r="P14" s="71"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E15" s="43"/>
-      <c r="F15" s="60">
+      <c r="E15" s="38"/>
+      <c r="F15" s="55">
         <v>8002</v>
       </c>
-      <c r="G15" s="83" t="s">
-        <v>143</v>
-      </c>
-      <c r="H15" s="60" t="s">
+      <c r="G15" s="78" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="67">
+      <c r="I15" s="62">
         <v>12</v>
       </c>
-      <c r="J15" s="67">
+      <c r="J15" s="62">
         <v>48</v>
       </c>
-      <c r="K15" s="71">
+      <c r="K15" s="66">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="L15" s="60" t="s">
+      <c r="L15" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="60">
+      <c r="M15" s="55">
         <v>50</v>
       </c>
-      <c r="N15" s="60">
+      <c r="N15" s="55">
         <v>40</v>
       </c>
-      <c r="O15" s="71"/>
-      <c r="P15" s="71"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E16" s="43"/>
-      <c r="F16" s="59">
+      <c r="E16" s="38"/>
+      <c r="F16" s="54">
         <v>9001</v>
       </c>
-      <c r="G16" s="82" t="s">
-        <v>144</v>
-      </c>
-      <c r="H16" s="59" t="s">
+      <c r="G16" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="H16" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="66">
+      <c r="I16" s="61">
         <v>12</v>
       </c>
-      <c r="J16" s="66">
+      <c r="J16" s="61">
         <v>12</v>
       </c>
-      <c r="K16" s="70">
+      <c r="K16" s="65">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="L16" s="59" t="s">
+      <c r="L16" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="59">
+      <c r="M16" s="54">
         <v>80</v>
       </c>
-      <c r="N16" s="59">
+      <c r="N16" s="54">
         <v>120</v>
       </c>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="69"/>
     </row>
     <row r="17" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E17" s="43"/>
-      <c r="F17" s="59">
+      <c r="E17" s="38"/>
+      <c r="F17" s="54">
         <v>9002</v>
       </c>
-      <c r="G17" s="82" t="s">
-        <v>145</v>
-      </c>
-      <c r="H17" s="59" t="s">
+      <c r="G17" s="77" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="66">
+      <c r="I17" s="61">
         <v>36</v>
       </c>
-      <c r="J17" s="66">
+      <c r="J17" s="61">
         <v>36</v>
       </c>
-      <c r="K17" s="70">
+      <c r="K17" s="65">
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-      <c r="L17" s="59" t="s">
+      <c r="L17" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="59">
+      <c r="M17" s="54">
         <v>80</v>
       </c>
-      <c r="N17" s="59">
+      <c r="N17" s="54">
         <v>20</v>
       </c>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="69"/>
     </row>
     <row r="18" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="43"/>
-      <c r="F18" s="61">
+      <c r="E18" s="38"/>
+      <c r="F18" s="56">
         <v>9003</v>
       </c>
-      <c r="G18" s="84" t="s">
-        <v>146</v>
-      </c>
-      <c r="H18" s="61" t="s">
+      <c r="G18" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="H18" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="68">
+      <c r="I18" s="63">
         <v>20</v>
       </c>
-      <c r="J18" s="68">
+      <c r="J18" s="63">
         <v>60</v>
       </c>
-      <c r="K18" s="72">
+      <c r="K18" s="67">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="L18" s="61" t="s">
+      <c r="L18" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="61">
+      <c r="M18" s="56">
         <v>80</v>
       </c>
-      <c r="N18" s="61">
+      <c r="N18" s="56">
         <v>10</v>
       </c>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
+      <c r="O18" s="70"/>
+      <c r="P18" s="70"/>
     </row>
     <row r="19" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="43"/>
+      <c r="E19" s="38"/>
       <c r="M19" s="29"/>
     </row>
     <row r="20" spans="5:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="43"/>
-      <c r="F20" s="78" t="s">
+      <c r="E20" s="38"/>
+      <c r="F20" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="78" t="s">
+      <c r="G20" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="78" t="s">
+      <c r="H20" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="64" t="s">
+      <c r="I20" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="J20" s="64" t="s">
+      <c r="J20" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="80" t="s">
-        <v>108</v>
-      </c>
-      <c r="L20" s="43"/>
+      <c r="K20" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="L20" s="38"/>
     </row>
     <row r="21" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E21" s="43"/>
-      <c r="F21" s="76">
+      <c r="E21" s="38"/>
+      <c r="F21" s="71">
         <v>100</v>
       </c>
-      <c r="G21" s="81" t="s">
+      <c r="G21" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="76" t="s">
+      <c r="H21" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="65">
+      <c r="I21" s="60">
         <v>21</v>
       </c>
-      <c r="J21" s="65">
+      <c r="J21" s="60">
         <v>2.5</v>
       </c>
-      <c r="K21" s="76">
+      <c r="K21" s="71">
         <v>1.3</v>
       </c>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
     </row>
     <row r="22" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E22" s="43"/>
-      <c r="F22" s="59">
+      <c r="E22" s="38"/>
+      <c r="F22" s="54">
         <v>200</v>
       </c>
-      <c r="G22" s="82" t="s">
+      <c r="G22" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="59" t="s">
+      <c r="H22" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="66">
+      <c r="I22" s="61">
         <v>21</v>
       </c>
-      <c r="J22" s="66">
+      <c r="J22" s="61">
         <v>3</v>
       </c>
-      <c r="K22" s="59">
+      <c r="K22" s="54">
         <v>2.5</v>
       </c>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="43"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
     </row>
     <row r="23" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E23" s="43"/>
-      <c r="F23" s="59">
+      <c r="E23" s="38"/>
+      <c r="F23" s="54">
         <v>300</v>
       </c>
-      <c r="G23" s="82" t="s">
+      <c r="G23" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="66">
+      <c r="I23" s="61">
         <v>21</v>
       </c>
-      <c r="J23" s="66">
+      <c r="J23" s="61">
         <v>1.3</v>
       </c>
-      <c r="K23" s="59">
+      <c r="K23" s="54">
         <v>2.5</v>
       </c>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
     </row>
     <row r="24" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E24" s="43"/>
-      <c r="F24" s="59">
+      <c r="E24" s="38"/>
+      <c r="F24" s="54">
         <v>500</v>
       </c>
-      <c r="G24" s="82" t="s">
+      <c r="G24" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="H24" s="59" t="s">
+      <c r="H24" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="66">
+      <c r="I24" s="61">
         <v>21</v>
       </c>
-      <c r="J24" s="66">
+      <c r="J24" s="61">
         <v>0.3</v>
       </c>
-      <c r="K24" s="59">
+      <c r="K24" s="54">
         <v>3.5</v>
       </c>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
     </row>
     <row r="25" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E25" s="43"/>
-      <c r="F25" s="59">
+      <c r="E25" s="38"/>
+      <c r="F25" s="54">
         <v>600</v>
       </c>
-      <c r="G25" s="82" t="s">
+      <c r="G25" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="59" t="s">
+      <c r="H25" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="66">
+      <c r="I25" s="61">
         <v>21</v>
       </c>
-      <c r="J25" s="66">
+      <c r="J25" s="61">
         <v>2</v>
       </c>
-      <c r="K25" s="59">
+      <c r="K25" s="54">
         <v>3.5</v>
       </c>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
     </row>
     <row r="26" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E26" s="43"/>
-      <c r="F26" s="60">
+      <c r="E26" s="38"/>
+      <c r="F26" s="55">
         <v>800</v>
       </c>
-      <c r="G26" s="83" t="s">
+      <c r="G26" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="60" t="s">
+      <c r="H26" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="67">
+      <c r="I26" s="62">
         <v>21</v>
       </c>
-      <c r="J26" s="67"/>
-      <c r="K26" s="71"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="66"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
     </row>
     <row r="27" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="43"/>
-      <c r="F27" s="61">
+      <c r="E27" s="38"/>
+      <c r="F27" s="56">
         <v>900</v>
       </c>
-      <c r="G27" s="84" t="s">
+      <c r="G27" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="63" t="s">
+      <c r="H27" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="68">
+      <c r="I27" s="63">
         <v>21</v>
       </c>
-      <c r="J27" s="68">
+      <c r="J27" s="63">
         <v>2.2999999999999998</v>
       </c>
-      <c r="K27" s="61">
+      <c r="K27" s="56">
         <v>3.5</v>
       </c>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
     </row>
     <row r="28" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="43"/>
+      <c r="E28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
     </row>
     <row r="29" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="43"/>
+      <c r="E29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2620,69 +2593,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12CEBBD-090D-4434-A119-3402FA7D8625}">
   <dimension ref="C2:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:E51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="8.375" customWidth="1"/>
-    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="70.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="33" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="34" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="7" t="s">
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="91" t="s">
         <v>48</v>
       </c>
       <c r="G5" s="30" t="s">
@@ -2690,23 +2663,23 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="7" t="s">
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="34" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94" t="s">
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="91" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="30" t="s">
@@ -2714,10 +2687,10 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="7" t="s">
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="91" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="30" t="s">
@@ -2725,10 +2698,10 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="7" t="s">
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="91" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="30" t="s">
@@ -2736,10 +2709,10 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="7" t="s">
+      <c r="C10" s="87"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="91" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="30" t="s">
@@ -2747,12 +2720,12 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94" t="s">
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="91" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="30" t="s">
@@ -2760,10 +2733,10 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="7" t="s">
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="91" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -2771,23 +2744,23 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="36" t="s">
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="91"/>
       <c r="G13" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94" t="s">
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="91" t="s">
         <v>48</v>
       </c>
       <c r="G14" s="30" t="s">
@@ -2795,30 +2768,30 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="7" t="s">
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="34" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="7"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="91"/>
       <c r="G16" s="30" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="7" t="s">
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="91" t="s">
         <v>48</v>
       </c>
       <c r="G17" s="30" t="s">
@@ -2826,114 +2799,114 @@
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="94"/>
-      <c r="D18" s="94" t="s">
+      <c r="C18" s="87"/>
+      <c r="D18" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="95" t="s">
+      <c r="E18" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="91"/>
       <c r="G18" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="7"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="91"/>
       <c r="G19" s="30" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="94" t="s">
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="91"/>
       <c r="G20" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="7"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="91"/>
       <c r="G21" s="30" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="7"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="91"/>
       <c r="G22" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94" t="s">
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="91"/>
       <c r="G23" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="94"/>
-      <c r="D24" s="94"/>
-      <c r="E24" s="94"/>
-      <c r="F24" s="7"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="91"/>
       <c r="G24" s="30" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="36" t="s">
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="91"/>
       <c r="G25" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="94" t="s">
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="91"/>
       <c r="G26" s="30" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
-      <c r="F27" s="37" t="s">
+      <c r="C27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="G27" s="35" t="s">
+      <c r="G27" s="34" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="94"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="37" t="s">
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="92" t="s">
         <v>48</v>
       </c>
       <c r="G28" s="30" t="s">
@@ -2941,21 +2914,21 @@
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="94"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="37"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="92"/>
       <c r="G29" s="30" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="94"/>
-      <c r="D30" s="94" t="s">
+      <c r="C30" s="87"/>
+      <c r="D30" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="94"/>
-      <c r="F30" s="37" t="s">
+      <c r="E30" s="87"/>
+      <c r="F30" s="92" t="s">
         <v>48</v>
       </c>
       <c r="G30" s="30" t="s">
@@ -2963,10 +2936,10 @@
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="94"/>
-      <c r="D31" s="94"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="37" t="s">
+      <c r="C31" s="87"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="92" t="s">
         <v>48</v>
       </c>
       <c r="G31" s="30" t="s">
@@ -2974,235 +2947,260 @@
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="94"/>
-      <c r="D32" s="94"/>
-      <c r="E32" s="94"/>
-      <c r="F32" s="37" t="s">
+      <c r="C32" s="87"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="34" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="94"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="37" t="s">
+      <c r="C33" s="87"/>
+      <c r="D33" s="87"/>
+      <c r="E33" s="87"/>
+      <c r="F33" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="G33" s="35" t="s">
+      <c r="G33" s="34" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="94"/>
-      <c r="D34" s="94"/>
-      <c r="E34" s="94"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="35" t="s">
+      <c r="C34" s="87"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="81" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" s="34" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="94"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="35" t="s">
+      <c r="C35" s="87"/>
+      <c r="D35" s="87"/>
+      <c r="E35" s="87"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="34" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
-      <c r="E36" s="94"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="35" t="s">
+      <c r="C36" s="87"/>
+      <c r="D36" s="87"/>
+      <c r="E36" s="87"/>
+      <c r="F36" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="94"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="35" t="s">
+      <c r="C37" s="87"/>
+      <c r="D37" s="87"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="35" t="s">
+      <c r="C38" s="87"/>
+      <c r="D38" s="87"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" s="34" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="94"/>
+      <c r="C39" s="87"/>
       <c r="D39" s="89" t="s">
         <v>76</v>
       </c>
       <c r="E39" s="89"/>
-      <c r="F39" s="37"/>
+      <c r="F39" s="81" t="s">
+        <v>48</v>
+      </c>
       <c r="G39" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="94"/>
+      <c r="C40" s="87"/>
       <c r="D40" s="89" t="s">
         <v>77</v>
       </c>
       <c r="E40" s="89"/>
-      <c r="F40" s="37"/>
+      <c r="F40" s="81" t="s">
+        <v>48</v>
+      </c>
       <c r="G40" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="C41" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="E41" t="s">
+      <c r="D41" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="F41" s="36"/>
-      <c r="G41" s="35" t="s">
+      <c r="E41" s="89"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="34" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="90" t="s">
+      <c r="C42" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="90" t="s">
+      <c r="D42" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="90"/>
-      <c r="F42" s="36" t="s">
+      <c r="E42" s="87"/>
+      <c r="F42" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G42" s="35" t="s">
+      <c r="G42" s="34" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="91"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="36" t="s">
+      <c r="C43" s="87"/>
+      <c r="D43" s="87"/>
+      <c r="E43" s="87"/>
+      <c r="F43" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G43" s="35" t="s">
+      <c r="G43" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="91"/>
-      <c r="D44" s="91"/>
-      <c r="E44" s="91"/>
-      <c r="F44" s="36" t="s">
+      <c r="C44" s="87"/>
+      <c r="D44" s="87"/>
+      <c r="E44" s="87"/>
+      <c r="F44" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G44" s="35" t="s">
+      <c r="G44" s="34" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="91"/>
-      <c r="D45" s="91"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="36" t="s">
+      <c r="C45" s="87"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G45" s="35" t="s">
+      <c r="G45" s="34" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="46" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="91"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="91"/>
-      <c r="F46" s="36" t="s">
+      <c r="C46" s="87"/>
+      <c r="D46" s="87"/>
+      <c r="E46" s="87"/>
+      <c r="F46" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G46" s="35" t="s">
+      <c r="G46" s="34" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="91"/>
-      <c r="D47" s="91"/>
-      <c r="E47" s="91"/>
-      <c r="F47" s="36" t="s">
+      <c r="C47" s="87"/>
+      <c r="D47" s="87"/>
+      <c r="E47" s="87"/>
+      <c r="F47" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G47" s="35" t="s">
+      <c r="G47" s="34" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="91"/>
-      <c r="D48" s="91"/>
-      <c r="E48" s="91"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="39" t="s">
+      <c r="C48" s="87"/>
+      <c r="D48" s="87"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="81"/>
+      <c r="G48" s="93" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="87"/>
+      <c r="D49" s="87"/>
+      <c r="E49" s="87"/>
+      <c r="F49" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" s="93" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="87"/>
+      <c r="D50" s="87"/>
+      <c r="E50" s="87"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="87"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="93" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C52" s="87"/>
+      <c r="D52" s="89" t="s">
+        <v>146</v>
+      </c>
+      <c r="E52" s="89"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="93" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="30" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="91"/>
-      <c r="D49" s="91"/>
-      <c r="E49" s="91"/>
-      <c r="F49" s="40" t="s">
+      <c r="D53" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="89"/>
+      <c r="F53" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="G49" s="39" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="91"/>
-      <c r="D50" s="91"/>
-      <c r="E50" s="91"/>
-      <c r="G50" s="29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="91"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
-      <c r="G51" s="41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="91"/>
-      <c r="D52" s="92" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" s="92"/>
-      <c r="G52" s="41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>105</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="G53" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="G53" s="41" t="s">
-        <v>107</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="C42:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D42:E51"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D53:E53"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="E7:E9"/>
@@ -3218,9 +3216,6 @@
     <mergeCell ref="D30:E38"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D40:E40"/>
-    <mergeCell ref="C42:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D42:E51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3237,17 +3232,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.75" customWidth="1"/>
-    <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TP-CASI TODAS LAS MODIFICACIONES
</commit_message>
<xml_diff>
--- a/SG - CLASES SEPARADAS/BASE DE DATOS.xlsx
+++ b/SG - CLASES SEPARADAS/BASE DE DATOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandra\Documents\GitHub\TP-GESTION-PROGRAMACION-2\SG - CLASES SEPARADAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A60D6BC0-34FB-4AC8-91FD-E0C007C4600A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F1617A31-E8C6-4F58-BD18-42EA5F5F9C98}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="1" activeTab="2" xr2:uid="{A683A0A2-948E-478E-9454-D16ED83D3AB7}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="148">
   <si>
     <t xml:space="preserve">PRECIO </t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>CIERRE DE CAJA</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1032,6 +1035,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1042,32 +1058,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1402,15 +1405,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1494,15 +1497,15 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -1634,12 +1637,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="88" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="85"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="90"/>
       <c r="E1" s="38"/>
       <c r="K1" s="37" t="s">
         <v>129</v>
@@ -1874,12 +1877,12 @@
       <c r="P6" s="54"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="85"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="90"/>
       <c r="E7" s="38"/>
       <c r="F7" s="54">
         <v>3001</v>
@@ -2593,8 +2596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12CEBBD-090D-4434-A119-3402FA7D8625}">
   <dimension ref="C2:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,13 +2612,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="31" t="s">
@@ -2635,16 +2638,16 @@
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="34" t="s">
@@ -2652,10 +2655,10 @@
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="91" t="s">
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G5" s="30" t="s">
@@ -2663,10 +2666,10 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="91" t="s">
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="34" t="s">
@@ -2674,12 +2677,12 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87" t="s">
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="91" t="s">
+      <c r="F7" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="30" t="s">
@@ -2687,10 +2690,10 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="91" t="s">
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="30" t="s">
@@ -2698,10 +2701,10 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="91" t="s">
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="30" t="s">
@@ -2709,10 +2712,10 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="87"/>
-      <c r="D10" s="87"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
       <c r="E10" s="81"/>
-      <c r="F10" s="91" t="s">
+      <c r="F10" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="30" t="s">
@@ -2720,12 +2723,12 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87" t="s">
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="91" t="s">
+      <c r="F11" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G11" s="30" t="s">
@@ -2733,10 +2736,10 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="91" t="s">
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -2744,23 +2747,23 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
       <c r="E13" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="91"/>
+      <c r="F13" s="83"/>
       <c r="G13" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87" t="s">
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="91" t="s">
+      <c r="F14" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G14" s="30" t="s">
@@ -2768,10 +2771,10 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="91" t="s">
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G15" s="34" t="s">
@@ -2779,19 +2782,19 @@
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="91"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="83"/>
       <c r="G16" s="30" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="91" t="s">
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="83" t="s">
         <v>48</v>
       </c>
       <c r="G17" s="30" t="s">
@@ -2799,103 +2802,117 @@
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="87"/>
-      <c r="D18" s="87" t="s">
+      <c r="C18" s="91"/>
+      <c r="D18" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="88" t="s">
+      <c r="E18" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="91"/>
+      <c r="F18" s="83" t="s">
+        <v>147</v>
+      </c>
       <c r="G18" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="87"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="83"/>
       <c r="G19" s="30" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87" t="s">
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="91"/>
+      <c r="F20" s="83"/>
       <c r="G20" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="87"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="83" t="s">
+        <v>147</v>
+      </c>
       <c r="G21" s="30" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="91"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="83" t="s">
+        <v>147</v>
+      </c>
       <c r="G22" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87" t="s">
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="91"/>
+      <c r="F23" s="83" t="s">
+        <v>147</v>
+      </c>
       <c r="G23" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="91"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="83" t="s">
+        <v>147</v>
+      </c>
       <c r="G24" s="30" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
       <c r="E25" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="91"/>
+      <c r="F25" s="83" t="s">
+        <v>147</v>
+      </c>
       <c r="G25" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="87" t="s">
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="91"/>
+      <c r="F26" s="83" t="s">
+        <v>147</v>
+      </c>
       <c r="G26" s="30" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="92" t="s">
+      <c r="C27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="84" t="s">
         <v>48</v>
       </c>
       <c r="G27" s="34" t="s">
@@ -2903,10 +2920,10 @@
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="92" t="s">
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="84" t="s">
         <v>48</v>
       </c>
       <c r="G28" s="30" t="s">
@@ -2914,21 +2931,21 @@
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="92"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="84"/>
       <c r="G29" s="30" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="87"/>
-      <c r="D30" s="87" t="s">
+      <c r="C30" s="91"/>
+      <c r="D30" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="87"/>
-      <c r="F30" s="92" t="s">
+      <c r="E30" s="91"/>
+      <c r="F30" s="84" t="s">
         <v>48</v>
       </c>
       <c r="G30" s="30" t="s">
@@ -2936,10 +2953,10 @@
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="92" t="s">
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="84" t="s">
         <v>48</v>
       </c>
       <c r="G31" s="30" t="s">
@@ -2947,10 +2964,10 @@
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="87"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="92" t="s">
+      <c r="C32" s="91"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="84" t="s">
         <v>48</v>
       </c>
       <c r="G32" s="34" t="s">
@@ -2958,10 +2975,10 @@
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="92" t="s">
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="84" t="s">
         <v>48</v>
       </c>
       <c r="G33" s="34" t="s">
@@ -2969,9 +2986,9 @@
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="91"/>
+      <c r="E34" s="91"/>
       <c r="F34" s="81" t="s">
         <v>48</v>
       </c>
@@ -2980,19 +2997,19 @@
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="87"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
+      <c r="C35" s="91"/>
+      <c r="D35" s="91"/>
+      <c r="E35" s="91"/>
       <c r="F35" s="36"/>
       <c r="G35" s="34" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="87"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="90" t="s">
+      <c r="C36" s="91"/>
+      <c r="D36" s="91"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="82" t="s">
         <v>48</v>
       </c>
       <c r="G36" s="34" t="s">
@@ -3000,10 +3017,10 @@
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="87"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="90" t="s">
+      <c r="C37" s="91"/>
+      <c r="D37" s="91"/>
+      <c r="E37" s="91"/>
+      <c r="F37" s="82" t="s">
         <v>48</v>
       </c>
       <c r="G37" s="34" t="s">
@@ -3011,10 +3028,10 @@
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="87"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="90" t="s">
+      <c r="C38" s="91"/>
+      <c r="D38" s="91"/>
+      <c r="E38" s="91"/>
+      <c r="F38" s="82" t="s">
         <v>48</v>
       </c>
       <c r="G38" s="34" t="s">
@@ -3022,11 +3039,11 @@
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="87"/>
-      <c r="D39" s="89" t="s">
+      <c r="C39" s="91"/>
+      <c r="D39" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="89"/>
+      <c r="E39" s="92"/>
       <c r="F39" s="81" t="s">
         <v>48</v>
       </c>
@@ -3035,11 +3052,11 @@
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="87"/>
-      <c r="D40" s="89" t="s">
+      <c r="C40" s="91"/>
+      <c r="D40" s="92" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="89"/>
+      <c r="E40" s="92"/>
       <c r="F40" s="81" t="s">
         <v>48</v>
       </c>
@@ -3051,23 +3068,25 @@
       <c r="C41" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="89" t="s">
+      <c r="D41" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="E41" s="89"/>
-      <c r="F41" s="35"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="G41" s="34" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="87" t="s">
+      <c r="C42" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="87" t="s">
+      <c r="D42" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="87"/>
+      <c r="E42" s="91"/>
       <c r="F42" s="35" t="s">
         <v>48</v>
       </c>
@@ -3076,9 +3095,9 @@
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="87"/>
-      <c r="D43" s="87"/>
-      <c r="E43" s="87"/>
+      <c r="C43" s="91"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="91"/>
       <c r="F43" s="35" t="s">
         <v>48</v>
       </c>
@@ -3087,9 +3106,9 @@
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="87"/>
-      <c r="D44" s="87"/>
-      <c r="E44" s="87"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="91"/>
+      <c r="E44" s="91"/>
       <c r="F44" s="35" t="s">
         <v>48</v>
       </c>
@@ -3098,9 +3117,9 @@
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="87"/>
-      <c r="D45" s="87"/>
-      <c r="E45" s="87"/>
+      <c r="C45" s="91"/>
+      <c r="D45" s="91"/>
+      <c r="E45" s="91"/>
       <c r="F45" s="35" t="s">
         <v>48</v>
       </c>
@@ -3109,9 +3128,9 @@
       </c>
     </row>
     <row r="46" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="87"/>
-      <c r="D46" s="87"/>
-      <c r="E46" s="87"/>
+      <c r="C46" s="91"/>
+      <c r="D46" s="91"/>
+      <c r="E46" s="91"/>
       <c r="F46" s="35" t="s">
         <v>48</v>
       </c>
@@ -3120,9 +3139,9 @@
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="87"/>
-      <c r="D47" s="87"/>
-      <c r="E47" s="87"/>
+      <c r="C47" s="91"/>
+      <c r="D47" s="91"/>
+      <c r="E47" s="91"/>
       <c r="F47" s="35" t="s">
         <v>48</v>
       </c>
@@ -3131,51 +3150,51 @@
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="87"/>
-      <c r="D48" s="87"/>
-      <c r="E48" s="87"/>
+      <c r="C48" s="91"/>
+      <c r="D48" s="91"/>
+      <c r="E48" s="91"/>
       <c r="F48" s="81"/>
-      <c r="G48" s="93" t="s">
+      <c r="G48" s="85" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="87"/>
-      <c r="D49" s="87"/>
-      <c r="E49" s="87"/>
-      <c r="F49" s="94" t="s">
+      <c r="C49" s="91"/>
+      <c r="D49" s="91"/>
+      <c r="E49" s="91"/>
+      <c r="F49" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="G49" s="93" t="s">
+      <c r="G49" s="85" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="87"/>
-      <c r="D50" s="87"/>
-      <c r="E50" s="87"/>
+      <c r="C50" s="91"/>
+      <c r="D50" s="91"/>
+      <c r="E50" s="91"/>
       <c r="F50" s="30"/>
       <c r="G50" s="34" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="87"/>
-      <c r="D51" s="87"/>
-      <c r="E51" s="87"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
       <c r="F51" s="30"/>
-      <c r="G51" s="93" t="s">
+      <c r="G51" s="85" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="87"/>
-      <c r="D52" s="89" t="s">
+      <c r="C52" s="91"/>
+      <c r="D52" s="92" t="s">
         <v>146</v>
       </c>
-      <c r="E52" s="89"/>
+      <c r="E52" s="92"/>
       <c r="F52" s="30"/>
-      <c r="G52" s="93" t="s">
+      <c r="G52" s="85" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3183,24 +3202,19 @@
       <c r="C53" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="D53" s="89" t="s">
+      <c r="D53" s="92" t="s">
         <v>105</v>
       </c>
-      <c r="E53" s="89"/>
+      <c r="E53" s="92"/>
       <c r="F53" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="G53" s="93" t="s">
+      <c r="G53" s="85" t="s">
         <v>106</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C42:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D42:E51"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D53:E53"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="E7:E9"/>
@@ -3216,6 +3230,11 @@
     <mergeCell ref="D30:E38"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="D40:E40"/>
+    <mergeCell ref="C42:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D42:E51"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D53:E53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Interfaz recuadros, acentos y stock critico 0
</commit_message>
<xml_diff>
--- a/SG - CLASES SEPARADAS/BASE DE DATOS.xlsx
+++ b/SG - CLASES SEPARADAS/BASE DE DATOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandra\Documents\GitHub\TP-GESTION-PROGRAMACION-2\SG - CLASES SEPARADAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0179E6CE-D6D7-4C8A-ABE7-0D002817E439}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9AA2AB2B-8EA2-46EE-8075-BEE2FBF7B554}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" firstSheet="1" activeTab="2" xr2:uid="{A683A0A2-948E-478E-9454-D16ED83D3AB7}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="150">
   <si>
     <t xml:space="preserve">PRECIO </t>
   </si>
@@ -465,9 +465,6 @@
     <t>CIERRE DE CAJA</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>descripcion</t>
   </si>
   <si>
@@ -475,6 +472,12 @@
   </si>
   <si>
     <t>LEYENDAS DE OPCIONES METODOS DE PAGO</t>
+  </si>
+  <si>
+    <t>MODIFICAR PROVEEDOR</t>
+  </si>
+  <si>
+    <t>MODIFICAR RETENCIONES -&gt;INTERFAZ (se superponen lineas retenciones)</t>
   </si>
 </sst>
 </file>
@@ -828,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1031,20 +1034,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1053,33 +1060,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1414,15 +1399,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1506,15 +1491,15 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="90" t="s">
+      <c r="A7" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -1622,7 +1607,7 @@
   <dimension ref="B1:Q29"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="G5" sqref="G5:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,12 +1631,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="93"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="87"/>
       <c r="F1" s="37"/>
       <c r="L1" s="36" t="s">
         <v>127</v>
@@ -1674,8 +1659,8 @@
       <c r="G2" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="85" t="s">
-        <v>146</v>
+      <c r="H2" s="82" t="s">
+        <v>145</v>
       </c>
       <c r="I2" s="72" t="s">
         <v>26</v>
@@ -1886,12 +1871,12 @@
       <c r="Q6" s="53"/>
     </row>
     <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="93"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="37"/>
       <c r="G7" s="53">
         <v>3001</v>
@@ -2603,10 +2588,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F12CEBBD-090D-4434-A119-3402FA7D8625}">
-  <dimension ref="C2:G54"/>
+  <dimension ref="C2:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,13 +2606,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="31" t="s">
@@ -2647,16 +2632,16 @@
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G4" s="34" t="s">
@@ -2664,10 +2649,10 @@
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="81" t="s">
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G5" s="30" t="s">
@@ -2675,10 +2660,10 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="81" t="s">
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="34" t="s">
@@ -2686,12 +2671,12 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95" t="s">
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="81" t="s">
+      <c r="F7" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G7" s="30" t="s">
@@ -2699,10 +2684,10 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="81" t="s">
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G8" s="30" t="s">
@@ -2710,10 +2695,10 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="81" t="s">
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G9" s="30" t="s">
@@ -2721,10 +2706,10 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
       <c r="E10" s="79"/>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G10" s="30" t="s">
@@ -2732,12 +2717,12 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95" t="s">
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="81" t="s">
+      <c r="F11" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G11" s="30" t="s">
@@ -2745,10 +2730,10 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="81" t="s">
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -2756,12 +2741,12 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
       <c r="E13" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G13" s="30" t="s">
@@ -2769,12 +2754,12 @@
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="95" t="s">
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="81" t="s">
+      <c r="F14" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G14" s="30" t="s">
@@ -2782,10 +2767,10 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="81" t="s">
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G15" s="34" t="s">
@@ -2793,21 +2778,21 @@
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="G16" s="89" t="s">
+      <c r="C16" s="88"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="83" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="81" t="s">
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G17" s="30" t="s">
@@ -2815,121 +2800,121 @@
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="95"/>
-      <c r="D18" s="95" t="s">
+      <c r="C18" s="88"/>
+      <c r="D18" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="96" t="s">
+      <c r="E18" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="81" t="s">
-        <v>145</v>
+      <c r="F18" s="80" t="s">
+        <v>47</v>
       </c>
       <c r="G18" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="81" t="s">
-        <v>145</v>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="80" t="s">
+        <v>47</v>
       </c>
       <c r="G19" s="30" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95" t="s">
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="81" t="s">
-        <v>145</v>
+      <c r="F20" s="80" t="s">
+        <v>47</v>
       </c>
       <c r="G20" s="30" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="95"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="81" t="s">
-        <v>145</v>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="80" t="s">
+        <v>47</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="81" t="s">
-        <v>145</v>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="80" t="s">
+        <v>47</v>
       </c>
       <c r="G22" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95" t="s">
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="81" t="s">
-        <v>145</v>
+      <c r="F23" s="80" t="s">
+        <v>47</v>
       </c>
       <c r="G23" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="81" t="s">
-        <v>145</v>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="80" t="s">
+        <v>47</v>
       </c>
       <c r="G24" s="30" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
       <c r="E25" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="81" t="s">
-        <v>145</v>
+      <c r="F25" s="80" t="s">
+        <v>47</v>
       </c>
       <c r="G25" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="81" t="s">
-        <v>145</v>
+      <c r="C26" s="88"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="80" t="s">
+        <v>47</v>
       </c>
       <c r="G26" s="30" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="82" t="s">
+      <c r="C27" s="88"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G27" s="34" t="s">
@@ -2937,10 +2922,10 @@
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="95"/>
-      <c r="D28" s="95"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="82" t="s">
+      <c r="C28" s="88"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G28" s="30" t="s">
@@ -2948,148 +2933,144 @@
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="82" t="s">
-        <v>145</v>
-      </c>
-      <c r="G29" s="89" t="s">
+      <c r="C29" s="88"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="83" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="95"/>
-      <c r="D30" s="95" t="s">
+      <c r="C30" s="88"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="88"/>
+      <c r="D31" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="95"/>
-      <c r="F30" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="G30" s="30" t="s">
+      <c r="E31" s="88"/>
+      <c r="F31" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" s="30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" s="30" t="s">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="30" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="95"/>
-      <c r="D32" s="95"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="G32" s="34" t="s">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="88"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" s="34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="95"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33" s="34" t="s">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="34" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="95"/>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="86" t="s">
-        <v>47</v>
-      </c>
-      <c r="G34" s="34" t="s">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="34" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="95"/>
-      <c r="D35" s="95"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="G35" s="34" t="s">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="88"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="95"/>
-      <c r="D36" s="95"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="G36" s="34" t="s">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="88"/>
+      <c r="D37" s="88"/>
+      <c r="E37" s="88"/>
+      <c r="F37" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="34" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="95"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="G37" s="34" t="s">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="88"/>
+      <c r="D38" s="88"/>
+      <c r="E38" s="88"/>
+      <c r="F38" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="95"/>
-      <c r="D38" s="95"/>
-      <c r="E38" s="95"/>
-      <c r="F38" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="G38" s="34" t="s">
-        <v>147</v>
-      </c>
-    </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="95"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="88"/>
+      <c r="E39" s="88"/>
       <c r="F39" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G39" s="34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="88"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="88"/>
+      <c r="F40" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="95"/>
-      <c r="D40" s="97" t="s">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="88"/>
+      <c r="D41" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="97"/>
-      <c r="F40" s="86" t="s">
-        <v>47</v>
-      </c>
-      <c r="G40" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="95"/>
-      <c r="D41" s="97" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="97"/>
-      <c r="F41" s="86" t="s">
+      <c r="E41" s="89"/>
+      <c r="F41" s="80" t="s">
         <v>47</v>
       </c>
       <c r="G41" s="30" t="s">
@@ -3097,184 +3078,197 @@
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="88"/>
+      <c r="D42" s="89" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="89"/>
+      <c r="F42" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="D42" s="97" t="s">
+      <c r="D43" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="E42" s="97"/>
-      <c r="F42" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G42" s="34" t="s">
+      <c r="E43" s="89"/>
+      <c r="F43" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="34" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="95" t="s">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="D43" s="95" t="s">
+      <c r="D44" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="95"/>
-      <c r="F43" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G43" s="34" t="s">
+      <c r="E44" s="88"/>
+      <c r="F44" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="34" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="95"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G44" s="34" t="s">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="88"/>
+      <c r="D45" s="88"/>
+      <c r="E45" s="88"/>
+      <c r="F45" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="34" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="95"/>
-      <c r="D45" s="95"/>
-      <c r="E45" s="95"/>
-      <c r="F45" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G45" s="34" t="s">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="88"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="88"/>
+      <c r="F46" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" s="34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="95"/>
-      <c r="D46" s="95"/>
-      <c r="E46" s="95"/>
-      <c r="F46" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G46" s="34" t="s">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="88"/>
+      <c r="D47" s="88"/>
+      <c r="E47" s="88"/>
+      <c r="F47" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" s="34" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="95"/>
-      <c r="D47" s="95"/>
-      <c r="E47" s="95"/>
-      <c r="F47" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G47" s="34" t="s">
+    <row r="48" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="88"/>
+      <c r="D48" s="88"/>
+      <c r="E48" s="88"/>
+      <c r="F48" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" s="34" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="95"/>
-      <c r="D48" s="95"/>
-      <c r="E48" s="95"/>
-      <c r="F48" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="G48" s="34" t="s">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="88"/>
+      <c r="D49" s="88"/>
+      <c r="E49" s="88"/>
+      <c r="F49" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="95"/>
-      <c r="D49" s="95"/>
-      <c r="E49" s="95"/>
-      <c r="F49" s="86" t="s">
-        <v>47</v>
-      </c>
-      <c r="G49" s="83" t="s">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="88"/>
+      <c r="D50" s="88"/>
+      <c r="E50" s="88"/>
+      <c r="F50" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G50" s="81" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="95"/>
-      <c r="D50" s="95"/>
-      <c r="E50" s="95"/>
-      <c r="F50" s="84" t="s">
-        <v>47</v>
-      </c>
-      <c r="G50" s="83" t="s">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="88"/>
+      <c r="D51" s="88"/>
+      <c r="E51" s="88"/>
+      <c r="F51" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" s="81" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="95"/>
-      <c r="D51" s="95"/>
-      <c r="E51" s="95"/>
-      <c r="F51" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="G51" s="34" t="s">
-        <v>148</v>
-      </c>
-    </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="95"/>
-      <c r="D52" s="95"/>
-      <c r="E52" s="95"/>
-      <c r="F52" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="G52" s="83" t="s">
+      <c r="C52" s="88"/>
+      <c r="D52" s="88"/>
+      <c r="E52" s="88"/>
+      <c r="F52" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G52" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="88"/>
+      <c r="D53" s="88"/>
+      <c r="E53" s="88"/>
+      <c r="F53" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G53" s="81" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="95"/>
-      <c r="D53" s="97" t="s">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="88"/>
+      <c r="D54" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="97"/>
-      <c r="F53" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="G53" s="83" t="s">
+      <c r="E54" s="89"/>
+      <c r="F54" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G54" s="81" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="30" t="s">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="D54" s="97" t="s">
+      <c r="D55" s="89" t="s">
         <v>103</v>
       </c>
-      <c r="E54" s="97"/>
-      <c r="F54" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="G54" s="83" t="s">
+      <c r="E55" s="89"/>
+      <c r="F55" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" s="81" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C43:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D43:E52"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D54:E54"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="E14:E17"/>
     <mergeCell ref="D4:D17"/>
-    <mergeCell ref="C4:C41"/>
+    <mergeCell ref="C4:C42"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="D18:D29"/>
-    <mergeCell ref="D30:E39"/>
-    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="D18:D30"/>
+    <mergeCell ref="D31:E40"/>
     <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="C44:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D44:E53"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D55:E55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>